<commit_message>
Pushing Selenium Project with everything working
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prase\IdeaProjects\orangeHRMPrasenjit\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC25A697-A613-42BE-8AEB-3F88C22EDB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CB838E-2FE8-4694-BA5E-49719D95E6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>admin1234</t>
   </si>
   <si>
-    <t>orangehrm_hvarma</t>
-  </si>
-  <si>
     <t>This@test1</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>Hitendra</t>
+  </si>
+  <si>
+    <t>orangehrm_hverma</t>
   </si>
 </sst>
 </file>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" activeCellId="1" sqref="A2 H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +413,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -431,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF39C60-EC60-475B-9797-34669AB49518}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -439,10 +439,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>